<commit_message>
ART-687: all test cases implemented API modifications for CCP and GCR affecting lots of classes and test cases. It's now possible to set a specific starting date for pattern development and a 'delayed' ultimate.
</commit_message>
<xml_diff>
--- a/test/data/spreadsheets/ART-687-1-CODNoInPeriodStartPeriod.xlsx
+++ b/test/data/spreadsheets/ART-687-1-CODNoInPeriodStartPeriod.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="19035" windowHeight="11760" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="19032" windowHeight="11760" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Usage" sheetId="4" r:id="rId1"/>
@@ -55,12 +55,12 @@
     <definedName name="RiskUseFixedSeed" hidden="1">FALSE</definedName>
     <definedName name="RiskUseMultipleCPUs" hidden="1">FALSE</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="78">
   <si>
     <t>Start Date</t>
   </si>
@@ -303,11 +303,14 @@
   <si>
     <t>Future Payment</t>
   </si>
+  <si>
+    <t>ultimate</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="6">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
@@ -316,7 +319,7 @@
     <numFmt numFmtId="167" formatCode="0.0%"/>
     <numFmt numFmtId="168" formatCode="#,##0.00;\(#,##0.00\);\-"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -378,16 +381,15 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -543,10 +545,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="8" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
@@ -554,21 +556,26 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Dezimal" xfId="2" builtinId="3"/>
+    <cellStyle name="Komma" xfId="2" builtinId="3"/>
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -642,6 +649,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -676,6 +684,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -851,34 +860,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="B2:P60"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="14.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13" style="2" customWidth="1"/>
     <col min="11" max="12" width="13" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" style="30"/>
+    <col min="15" max="15" width="9.109375" style="30"/>
   </cols>
   <sheetData>
-    <row r="2" spans="5:16">
+    <row r="2" spans="5:16" x14ac:dyDescent="0.3">
       <c r="E2" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="5:16">
+    <row r="3" spans="5:16" x14ac:dyDescent="0.3">
       <c r="E3" s="1" t="s">
         <v>0</v>
       </c>
@@ -886,7 +895,7 @@
         <v>40544</v>
       </c>
     </row>
-    <row r="4" spans="5:16">
+    <row r="4" spans="5:16" x14ac:dyDescent="0.3">
       <c r="E4" s="1" t="s">
         <v>5</v>
       </c>
@@ -900,7 +909,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="5:16">
+    <row r="5" spans="5:16" x14ac:dyDescent="0.3">
       <c r="E5" s="1" t="s">
         <v>65</v>
       </c>
@@ -911,10 +920,10 @@
       <c r="N5" s="13"/>
       <c r="O5" s="31"/>
     </row>
-    <row r="6" spans="5:16">
+    <row r="6" spans="5:16" x14ac:dyDescent="0.3">
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="5:16">
+    <row r="7" spans="5:16" x14ac:dyDescent="0.3">
       <c r="E7" s="8" t="s">
         <v>15</v>
       </c>
@@ -924,7 +933,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="5:16">
+    <row r="8" spans="5:16" x14ac:dyDescent="0.3">
       <c r="E8" s="1" t="s">
         <v>20</v>
       </c>
@@ -935,7 +944,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="5:16">
+    <row r="9" spans="5:16" x14ac:dyDescent="0.3">
       <c r="E9" s="1" t="s">
         <v>12</v>
       </c>
@@ -946,7 +955,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="5:16">
+    <row r="10" spans="5:16" x14ac:dyDescent="0.3">
       <c r="E10" s="1" t="s">
         <v>71</v>
       </c>
@@ -957,7 +966,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="5:16">
+    <row r="11" spans="5:16" x14ac:dyDescent="0.3">
       <c r="E11" s="1" t="s">
         <v>13</v>
       </c>
@@ -969,7 +978,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="5:16">
+    <row r="13" spans="5:16" x14ac:dyDescent="0.3">
       <c r="E13" s="8" t="s">
         <v>16</v>
       </c>
@@ -980,7 +989,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="5:16">
+    <row r="14" spans="5:16" x14ac:dyDescent="0.3">
       <c r="E14" s="9" t="s">
         <v>2</v>
       </c>
@@ -999,7 +1008,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="5:16">
+    <row r="15" spans="5:16" x14ac:dyDescent="0.3">
       <c r="E15" s="16"/>
       <c r="F15" s="16"/>
       <c r="G15" s="17"/>
@@ -1010,7 +1019,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="5:16">
+    <row r="16" spans="5:16" x14ac:dyDescent="0.3">
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
       <c r="G16" s="17"/>
@@ -1021,7 +1030,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="5:16">
+    <row r="17" spans="5:16" x14ac:dyDescent="0.3">
       <c r="E17" s="16"/>
       <c r="F17" s="16"/>
       <c r="G17" s="17"/>
@@ -1032,7 +1041,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="5:16">
+    <row r="18" spans="5:16" x14ac:dyDescent="0.3">
       <c r="E18" s="16"/>
       <c r="F18" s="16"/>
       <c r="G18" s="17"/>
@@ -1043,12 +1052,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="5:16">
+    <row r="19" spans="5:16" x14ac:dyDescent="0.3">
       <c r="E19" s="18"/>
       <c r="F19" s="15"/>
       <c r="G19" s="19"/>
     </row>
-    <row r="20" spans="5:16">
+    <row r="20" spans="5:16" x14ac:dyDescent="0.3">
       <c r="E20" s="18"/>
       <c r="F20" s="15"/>
       <c r="G20" s="19"/>
@@ -1056,17 +1065,17 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="5:16">
+    <row r="21" spans="5:16" x14ac:dyDescent="0.3">
       <c r="E21" s="18"/>
       <c r="F21" s="15"/>
       <c r="G21" s="19"/>
     </row>
-    <row r="22" spans="5:16">
+    <row r="22" spans="5:16" x14ac:dyDescent="0.3">
       <c r="O22" s="30" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="5:16">
+    <row r="23" spans="5:16" x14ac:dyDescent="0.3">
       <c r="E23" s="8" t="s">
         <v>18</v>
       </c>
@@ -1075,14 +1084,14 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="5:16">
+    <row r="24" spans="5:16" x14ac:dyDescent="0.3">
       <c r="E24" s="8"/>
       <c r="F24" s="4"/>
       <c r="P24" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="5:16">
+    <row r="25" spans="5:16" x14ac:dyDescent="0.3">
       <c r="E25" s="8" t="s">
         <v>29</v>
       </c>
@@ -1091,14 +1100,14 @@
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="5:16">
+    <row r="26" spans="5:16" x14ac:dyDescent="0.3">
       <c r="E26" s="8"/>
       <c r="F26" s="4"/>
       <c r="O26" s="30" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="5:16">
+    <row r="27" spans="5:16" x14ac:dyDescent="0.3">
       <c r="E27" s="1" t="s">
         <v>28</v>
       </c>
@@ -1110,7 +1119,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="5:16">
+    <row r="28" spans="5:16" x14ac:dyDescent="0.3">
       <c r="E28" s="1" t="s">
         <v>19</v>
       </c>
@@ -1125,7 +1134,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="5:16">
+    <row r="29" spans="5:16" x14ac:dyDescent="0.3">
       <c r="E29" s="1" t="s">
         <v>7</v>
       </c>
@@ -1137,21 +1146,21 @@
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="5:16">
+    <row r="30" spans="5:16" x14ac:dyDescent="0.3">
       <c r="E30" s="8"/>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="5:16">
+    <row r="31" spans="5:16" x14ac:dyDescent="0.3">
       <c r="E31" s="8" t="s">
         <v>30</v>
       </c>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="5:16">
+    <row r="32" spans="5:16" x14ac:dyDescent="0.3">
       <c r="E32" s="8"/>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="2:12">
+    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
       <c r="E33" s="1" t="s">
         <v>65</v>
       </c>
@@ -1160,10 +1169,10 @@
         <v>40699</v>
       </c>
     </row>
-    <row r="34" spans="2:12">
+    <row r="34" spans="2:12" x14ac:dyDescent="0.3">
       <c r="F34" s="4"/>
     </row>
-    <row r="35" spans="2:12">
+    <row r="35" spans="2:12" x14ac:dyDescent="0.3">
       <c r="E35" s="8"/>
       <c r="F35" s="4" t="s">
         <v>33</v>
@@ -1175,7 +1184,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="2:12">
+    <row r="36" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B36" s="28" t="s">
         <v>46</v>
       </c>
@@ -1211,7 +1220,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="37" spans="2:12">
+    <row r="37" spans="2:12" x14ac:dyDescent="0.3">
       <c r="E37" s="1" t="s">
         <v>35</v>
       </c>
@@ -1244,7 +1253,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="38" spans="2:12">
+    <row r="38" spans="2:12" x14ac:dyDescent="0.3">
       <c r="F38" s="5"/>
       <c r="G38" s="22"/>
       <c r="H38" s="7"/>
@@ -1253,7 +1262,7 @@
       <c r="K38" s="22"/>
       <c r="L38" s="22"/>
     </row>
-    <row r="39" spans="2:12">
+    <row r="39" spans="2:12" x14ac:dyDescent="0.3">
       <c r="E39" s="1" t="s">
         <v>35</v>
       </c>
@@ -1263,7 +1272,7 @@
       </c>
       <c r="G39" s="34"/>
     </row>
-    <row r="40" spans="2:12">
+    <row r="40" spans="2:12" x14ac:dyDescent="0.3">
       <c r="F40" s="5"/>
       <c r="G40" s="22"/>
       <c r="H40" s="7"/>
@@ -1272,7 +1281,7 @@
       <c r="K40" s="22"/>
       <c r="L40" s="22"/>
     </row>
-    <row r="41" spans="2:12">
+    <row r="41" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B41" s="28" t="s">
         <v>47</v>
       </c>
@@ -1292,7 +1301,7 @@
       <c r="K41" s="22"/>
       <c r="L41" s="22"/>
     </row>
-    <row r="42" spans="2:12">
+    <row r="42" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B42" s="28" t="s">
         <v>48</v>
       </c>
@@ -1312,7 +1321,7 @@
       <c r="K42" s="22"/>
       <c r="L42" s="22"/>
     </row>
-    <row r="43" spans="2:12">
+    <row r="43" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B43" s="28" t="s">
         <v>49</v>
       </c>
@@ -1332,7 +1341,7 @@
       <c r="K43" s="22"/>
       <c r="L43" s="22"/>
     </row>
-    <row r="45" spans="2:12">
+    <row r="45" spans="2:12" x14ac:dyDescent="0.3">
       <c r="F45" s="2" t="s">
         <v>9</v>
       </c>
@@ -1355,7 +1364,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="2:12">
+    <row r="46" spans="2:12" x14ac:dyDescent="0.3">
       <c r="E46" s="2" t="s">
         <v>22</v>
       </c>
@@ -1381,7 +1390,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="2:12" ht="6" customHeight="1">
+    <row r="47" spans="2:12" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E47" s="2"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
@@ -1389,7 +1398,7 @@
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
     </row>
-    <row r="48" spans="2:12">
+    <row r="48" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B48" s="28" t="s">
         <v>60</v>
       </c>
@@ -1424,7 +1433,7 @@
         <v>3600.0000000000009</v>
       </c>
     </row>
-    <row r="49" spans="5:12">
+    <row r="49" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E49" s="33">
         <f>E48+12</f>
         <v>27</v>
@@ -1457,7 +1466,7 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="50" spans="5:12">
+    <row r="50" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E50" s="33">
         <v>43</v>
       </c>
@@ -1489,7 +1498,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="51" spans="5:12">
+    <row r="51" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E51" s="33">
         <f t="shared" ref="E51:E58" si="5">E50+12</f>
         <v>55</v>
@@ -1522,7 +1531,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="52" spans="5:12">
+    <row r="52" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E52" s="33">
         <f t="shared" si="5"/>
         <v>67</v>
@@ -1555,7 +1564,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="53" spans="5:12">
+    <row r="53" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E53" s="33">
         <f t="shared" si="5"/>
         <v>79</v>
@@ -1588,7 +1597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="5:12">
+    <row r="54" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E54" s="33">
         <f t="shared" si="5"/>
         <v>91</v>
@@ -1621,7 +1630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="5:12">
+    <row r="55" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E55" s="33">
         <f t="shared" si="5"/>
         <v>103</v>
@@ -1654,7 +1663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="5:12">
+    <row r="56" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E56" s="33">
         <f t="shared" si="5"/>
         <v>115</v>
@@ -1687,7 +1696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="5:12">
+    <row r="57" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E57" s="33">
         <f t="shared" si="5"/>
         <v>127</v>
@@ -1720,7 +1729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="5:12">
+    <row r="58" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E58" s="33">
         <f t="shared" si="5"/>
         <v>139</v>
@@ -1753,11 +1762,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="5:12">
+    <row r="59" spans="5:12" x14ac:dyDescent="0.3">
       <c r="J59" s="1"/>
       <c r="K59" s="2"/>
     </row>
-    <row r="60" spans="5:12">
+    <row r="60" spans="5:12" x14ac:dyDescent="0.3">
       <c r="J60" s="1"/>
       <c r="K60" s="35">
         <f ca="1">SUM(K48:K58)</f>
@@ -1780,20 +1789,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="37" t="s">
         <v>22</v>
       </c>
@@ -1801,7 +1810,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="39">
         <f>Usage!E48</f>
         <v>15</v>
@@ -1811,7 +1820,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="39">
         <f>Usage!E49</f>
         <v>27</v>
@@ -1821,7 +1830,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="39">
         <f>Usage!E50</f>
         <v>43</v>
@@ -1831,7 +1840,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="39">
         <f>Usage!E51</f>
         <v>55</v>
@@ -1841,7 +1850,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="39">
         <f>Usage!E52</f>
         <v>67</v>
@@ -1857,16 +1866,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="37" t="s">
         <v>72</v>
       </c>
@@ -1886,19 +1895,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>75</v>
       </c>
@@ -1906,15 +1915,18 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="43">
-        <v>40543</v>
-      </c>
-      <c r="B2" s="44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="40">
+        <v>40699</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="40">
         <v>41156</v>
       </c>
@@ -1922,7 +1934,7 @@
         <v>3600.0000000000009</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="40">
         <v>41521</v>
       </c>
@@ -1930,15 +1942,15 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="43">
-        <v>41521</v>
-      </c>
-      <c r="B5" s="44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="44">
+        <v>41640</v>
+      </c>
+      <c r="B5" s="43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="40">
         <v>42008</v>
       </c>
@@ -1946,7 +1958,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="41">
         <v>42373</v>
       </c>
@@ -1954,7 +1966,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="41">
         <v>42739</v>
       </c>
@@ -1964,5 +1976,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Prepare an initial version of the artisan 2 model.
</commit_message>
<xml_diff>
--- a/test/data/spreadsheets/ART-687-1-CODNoInPeriodStartPeriod.xlsx
+++ b/test/data/spreadsheets/ART-687-1-CODNoInPeriodStartPeriod.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="19032" windowHeight="11760" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="19035" windowHeight="11760" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Usage" sheetId="4" r:id="rId1"/>
@@ -55,7 +55,7 @@
     <definedName name="RiskUseFixedSeed" hidden="1">FALSE</definedName>
     <definedName name="RiskUseMultipleCPUs" hidden="1">FALSE</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -310,16 +310,16 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
-    <numFmt numFmtId="165" formatCode="_-#,##0_-;_-\(#,##0\)_-;_-* &quot;-&quot;??_-"/>
-    <numFmt numFmtId="166" formatCode="_-#,##0.00_-;_-\(#,##0.00\)_-;_-* &quot;-&quot;??_-"/>
-    <numFmt numFmtId="167" formatCode="0.0%"/>
-    <numFmt numFmtId="168" formatCode="#,##0.00;\(#,##0.00\);\-"/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="166" formatCode="_-#,##0_-;_-\(#,##0\)_-;_-* &quot;-&quot;??_-"/>
+    <numFmt numFmtId="167" formatCode="_-#,##0.00_-;_-\(#,##0.00\)_-;_-* &quot;-&quot;??_-"/>
+    <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="169" formatCode="#,##0.00;\(#,##0.00\);\-"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -388,12 +388,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -442,9 +436,9 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -455,114 +449,112 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="8" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Komma" xfId="2" builtinId="3"/>
-    <cellStyle name="Prozent" xfId="1" builtinId="5"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -575,9 +567,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -615,7 +607,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -649,7 +641,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -684,10 +675,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -860,7 +850,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
@@ -870,24 +860,24 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="14.5546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13" style="2" customWidth="1"/>
     <col min="11" max="12" width="13" customWidth="1"/>
-    <col min="15" max="15" width="9.109375" style="30"/>
+    <col min="15" max="15" width="9.140625" style="30"/>
   </cols>
   <sheetData>
-    <row r="2" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="5:16">
       <c r="E2" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="5:16">
       <c r="E3" s="1" t="s">
         <v>0</v>
       </c>
@@ -895,7 +885,7 @@
         <v>40544</v>
       </c>
     </row>
-    <row r="4" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="5:16">
       <c r="E4" s="1" t="s">
         <v>5</v>
       </c>
@@ -909,7 +899,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="5:16">
       <c r="E5" s="1" t="s">
         <v>65</v>
       </c>
@@ -920,10 +910,10 @@
       <c r="N5" s="13"/>
       <c r="O5" s="31"/>
     </row>
-    <row r="6" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="5:16">
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="5:16">
       <c r="E7" s="8" t="s">
         <v>15</v>
       </c>
@@ -933,7 +923,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="5:16">
       <c r="E8" s="1" t="s">
         <v>20</v>
       </c>
@@ -944,7 +934,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="5:16">
       <c r="E9" s="1" t="s">
         <v>12</v>
       </c>
@@ -955,7 +945,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="5:16">
       <c r="E10" s="1" t="s">
         <v>71</v>
       </c>
@@ -966,7 +956,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="5:16">
       <c r="E11" s="1" t="s">
         <v>13</v>
       </c>
@@ -978,7 +968,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="5:16">
       <c r="E13" s="8" t="s">
         <v>16</v>
       </c>
@@ -989,7 +979,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="5:16">
       <c r="E14" s="9" t="s">
         <v>2</v>
       </c>
@@ -1008,7 +998,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="5:16">
       <c r="E15" s="16"/>
       <c r="F15" s="16"/>
       <c r="G15" s="17"/>
@@ -1019,7 +1009,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="5:16">
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
       <c r="G16" s="17"/>
@@ -1030,7 +1020,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:16">
       <c r="E17" s="16"/>
       <c r="F17" s="16"/>
       <c r="G17" s="17"/>
@@ -1041,7 +1031,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:16">
       <c r="E18" s="16"/>
       <c r="F18" s="16"/>
       <c r="G18" s="17"/>
@@ -1052,12 +1042,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="5:16">
       <c r="E19" s="18"/>
       <c r="F19" s="15"/>
       <c r="G19" s="19"/>
     </row>
-    <row r="20" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="5:16">
       <c r="E20" s="18"/>
       <c r="F20" s="15"/>
       <c r="G20" s="19"/>
@@ -1065,17 +1055,17 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="5:16">
       <c r="E21" s="18"/>
       <c r="F21" s="15"/>
       <c r="G21" s="19"/>
     </row>
-    <row r="22" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="5:16">
       <c r="O22" s="30" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="5:16">
       <c r="E23" s="8" t="s">
         <v>18</v>
       </c>
@@ -1084,14 +1074,14 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="5:16">
       <c r="E24" s="8"/>
       <c r="F24" s="4"/>
       <c r="P24" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="5:16">
       <c r="E25" s="8" t="s">
         <v>29</v>
       </c>
@@ -1100,14 +1090,14 @@
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="5:16">
       <c r="E26" s="8"/>
       <c r="F26" s="4"/>
       <c r="O26" s="30" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="5:16">
       <c r="E27" s="1" t="s">
         <v>28</v>
       </c>
@@ -1119,7 +1109,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="5:16">
       <c r="E28" s="1" t="s">
         <v>19</v>
       </c>
@@ -1134,7 +1124,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="5:16">
       <c r="E29" s="1" t="s">
         <v>7</v>
       </c>
@@ -1146,21 +1136,21 @@
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="5:16">
       <c r="E30" s="8"/>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="5:16">
       <c r="E31" s="8" t="s">
         <v>30</v>
       </c>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="5:16">
       <c r="E32" s="8"/>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:12">
       <c r="E33" s="1" t="s">
         <v>65</v>
       </c>
@@ -1169,10 +1159,10 @@
         <v>40699</v>
       </c>
     </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:12">
       <c r="F34" s="4"/>
     </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:12">
       <c r="E35" s="8"/>
       <c r="F35" s="4" t="s">
         <v>33</v>
@@ -1184,7 +1174,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:12">
       <c r="B36" s="28" t="s">
         <v>46</v>
       </c>
@@ -1220,7 +1210,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:12">
       <c r="E37" s="1" t="s">
         <v>35</v>
       </c>
@@ -1253,7 +1243,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:12">
       <c r="F38" s="5"/>
       <c r="G38" s="22"/>
       <c r="H38" s="7"/>
@@ -1262,7 +1252,7 @@
       <c r="K38" s="22"/>
       <c r="L38" s="22"/>
     </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:12">
       <c r="E39" s="1" t="s">
         <v>35</v>
       </c>
@@ -1272,7 +1262,7 @@
       </c>
       <c r="G39" s="34"/>
     </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:12">
       <c r="F40" s="5"/>
       <c r="G40" s="22"/>
       <c r="H40" s="7"/>
@@ -1281,7 +1271,7 @@
       <c r="K40" s="22"/>
       <c r="L40" s="22"/>
     </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:12">
       <c r="B41" s="28" t="s">
         <v>47</v>
       </c>
@@ -1301,7 +1291,7 @@
       <c r="K41" s="22"/>
       <c r="L41" s="22"/>
     </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:12">
       <c r="B42" s="28" t="s">
         <v>48</v>
       </c>
@@ -1321,7 +1311,7 @@
       <c r="K42" s="22"/>
       <c r="L42" s="22"/>
     </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:12">
       <c r="B43" s="28" t="s">
         <v>49</v>
       </c>
@@ -1341,7 +1331,7 @@
       <c r="K43" s="22"/>
       <c r="L43" s="22"/>
     </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:12">
       <c r="F45" s="2" t="s">
         <v>9</v>
       </c>
@@ -1364,7 +1354,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:12">
       <c r="E46" s="2" t="s">
         <v>22</v>
       </c>
@@ -1390,7 +1380,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="2:12" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:12" ht="6" customHeight="1">
       <c r="E47" s="2"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
@@ -1398,7 +1388,7 @@
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
     </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:12">
       <c r="B48" s="28" t="s">
         <v>60</v>
       </c>
@@ -1433,7 +1423,7 @@
         <v>3600.0000000000009</v>
       </c>
     </row>
-    <row r="49" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="5:12">
       <c r="E49" s="33">
         <f>E48+12</f>
         <v>27</v>
@@ -1466,7 +1456,7 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="50" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="5:12">
       <c r="E50" s="33">
         <v>43</v>
       </c>
@@ -1498,7 +1488,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="51" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="5:12">
       <c r="E51" s="33">
         <f t="shared" ref="E51:E58" si="5">E50+12</f>
         <v>55</v>
@@ -1531,7 +1521,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="52" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="5:12">
       <c r="E52" s="33">
         <f t="shared" si="5"/>
         <v>67</v>
@@ -1564,7 +1554,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="53" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="5:12">
       <c r="E53" s="33">
         <f t="shared" si="5"/>
         <v>79</v>
@@ -1597,7 +1587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="5:12">
       <c r="E54" s="33">
         <f t="shared" si="5"/>
         <v>91</v>
@@ -1630,7 +1620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="5:12">
       <c r="E55" s="33">
         <f t="shared" si="5"/>
         <v>103</v>
@@ -1663,7 +1653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="5:12">
       <c r="E56" s="33">
         <f t="shared" si="5"/>
         <v>115</v>
@@ -1696,7 +1686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="5:12">
       <c r="E57" s="33">
         <f t="shared" si="5"/>
         <v>127</v>
@@ -1729,7 +1719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="5:12">
       <c r="E58" s="33">
         <f t="shared" si="5"/>
         <v>139</v>
@@ -1762,11 +1752,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="5:12">
       <c r="J59" s="1"/>
       <c r="K59" s="2"/>
     </row>
-    <row r="60" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="5:12">
       <c r="J60" s="1"/>
       <c r="K60" s="35">
         <f ca="1">SUM(K48:K58)</f>
@@ -1789,20 +1779,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" s="37" t="s">
         <v>22</v>
       </c>
@@ -1810,7 +1800,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" s="39">
         <f>Usage!E48</f>
         <v>15</v>
@@ -1820,7 +1810,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" s="39">
         <f>Usage!E49</f>
         <v>27</v>
@@ -1830,7 +1820,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4" s="39">
         <f>Usage!E50</f>
         <v>43</v>
@@ -1840,7 +1830,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2">
       <c r="A5" s="39">
         <f>Usage!E51</f>
         <v>55</v>
@@ -1850,7 +1840,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2">
       <c r="A6" s="39">
         <f>Usage!E52</f>
         <v>67</v>
@@ -1866,16 +1856,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" s="37" t="s">
         <v>72</v>
       </c>
@@ -1895,19 +1885,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>75</v>
       </c>
@@ -1915,7 +1905,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" s="40">
         <v>40699</v>
       </c>
@@ -1926,7 +1916,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" s="40">
         <v>41156</v>
       </c>
@@ -1934,7 +1924,7 @@
         <v>3600.0000000000009</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" s="40">
         <v>41521</v>
       </c>
@@ -1942,35 +1932,27 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="44">
-        <v>41640</v>
-      </c>
-      <c r="B5" s="43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="40">
+    <row r="5" spans="1:3">
+      <c r="A5" s="40">
         <v>42008</v>
       </c>
+      <c r="B5">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="41">
+        <v>42373</v>
+      </c>
       <c r="B6">
-        <v>5400</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="41">
-        <v>42373</v>
+        <v>42739</v>
       </c>
       <c r="B7">
-        <v>3600</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="41">
-        <v>42739</v>
-      </c>
-      <c r="B8">
         <v>900</v>
       </c>
     </row>

</xml_diff>